<commit_message>
commit 1 using gtbash
</commit_message>
<xml_diff>
--- a/test_data/Facebook.xlsx
+++ b/test_data/Facebook.xlsx
@@ -1,17 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20403"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{72D631E8-7BBB-4D29-9971-A4567E324060}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="96" yWindow="60" windowWidth="22932" windowHeight="9504"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17172" windowHeight="3684" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1:I11"/>
 </workbook>
 </file>
 
@@ -75,8 +77,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -121,6 +123,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -167,7 +177,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -199,9 +209,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -233,6 +261,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -408,14 +454,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="34.6640625" customWidth="1"/>
     <col min="2" max="2" width="16.6640625" customWidth="1"/>
@@ -423,7 +469,7 @@
     <col min="4" max="4" width="27.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -455,7 +501,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -494,24 +540,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>